<commit_message>
Experiments defined for NARMA
</commit_message>
<xml_diff>
--- a/Lazy 8/Architecture.xlsx
+++ b/Lazy 8/Architecture.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B2839E1-609C-47D9-AD6C-E44669A8EFD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bweborg/Documents/Thesis/explore-esn/Lazy 8/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D7A1AC-DF81-5944-9814-D8EE4EA3A737}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28520" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Experiment</t>
   </si>
@@ -58,12 +63,6 @@
     <t>147B</t>
   </si>
   <si>
-    <t>148A</t>
-  </si>
-  <si>
-    <t>148B</t>
-  </si>
-  <si>
     <t>156A</t>
   </si>
   <si>
@@ -76,12 +75,6 @@
     <t>157B</t>
   </si>
   <si>
-    <t>158A</t>
-  </si>
-  <si>
-    <t>158B</t>
-  </si>
-  <si>
     <t>246A</t>
   </si>
   <si>
@@ -94,12 +87,6 @@
     <t>247B</t>
   </si>
   <si>
-    <t>248A</t>
-  </si>
-  <si>
-    <t>248B</t>
-  </si>
-  <si>
     <t>256A</t>
   </si>
   <si>
@@ -112,12 +99,6 @@
     <t>257B</t>
   </si>
   <si>
-    <t>258A</t>
-  </si>
-  <si>
-    <t>258B</t>
-  </si>
-  <si>
     <t>346A</t>
   </si>
   <si>
@@ -130,12 +111,6 @@
     <t>347B</t>
   </si>
   <si>
-    <t>348A</t>
-  </si>
-  <si>
-    <t>348B</t>
-  </si>
-  <si>
     <t>356A</t>
   </si>
   <si>
@@ -148,17 +123,35 @@
     <t>357B</t>
   </si>
   <si>
-    <t>358A</t>
-  </si>
-  <si>
-    <t>358B</t>
+    <t>846A</t>
+  </si>
+  <si>
+    <t>846B</t>
+  </si>
+  <si>
+    <t>847A</t>
+  </si>
+  <si>
+    <t>847B</t>
+  </si>
+  <si>
+    <t>856A</t>
+  </si>
+  <si>
+    <t>856B</t>
+  </si>
+  <si>
+    <t>857A</t>
+  </si>
+  <si>
+    <t>857B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,15 +499,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56:F61"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1469</v>
       </c>
@@ -554,7 +547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -574,7 +567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -594,7 +587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1479</v>
       </c>
@@ -614,7 +607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -634,7 +627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -654,9 +647,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>1489</v>
+        <v>1569</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -665,16 +658,16 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -685,16 +678,16 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -705,18 +698,18 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>1569</v>
+        <v>1579</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -728,13 +721,13 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -748,13 +741,13 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -768,135 +761,135 @@
         <v>2</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>1579</v>
+        <v>2469</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>1589</v>
+        <v>2479</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>2469</v>
+        <v>2569</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -905,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -914,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -925,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -934,7 +927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -945,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -954,9 +947,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>2479</v>
+        <v>2579</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -965,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -974,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -985,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -994,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -1005,7 +998,7 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1014,252 +1007,252 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>2482</v>
+        <v>3469</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>2569</v>
+        <v>3479</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>2579</v>
+        <v>3569</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>2</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34">
         <v>2</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>2589</v>
+        <v>3579</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <v>2</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
         <v>2</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37">
         <v>2</v>
       </c>
       <c r="E37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="1">
-        <v>3469</v>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>8469</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1274,12 +1267,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1294,12 +1287,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1314,12 +1307,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>3479</v>
+        <v>8479</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1334,12 +1327,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -1354,12 +1347,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1374,72 +1367,72 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>3489</v>
+        <v>8569</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F45">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F46">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>3569</v>
+        <v>8579</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1448,18 +1441,18 @@
         <v>2</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1468,18 +1461,18 @@
         <v>2</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -1488,129 +1481,9 @@
         <v>2</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="1">
-        <v>3579</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50">
-        <v>2</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <v>2</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>2</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="1">
-        <v>3589</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>2</v>
-      </c>
-      <c r="E53">
-        <v>2</v>
-      </c>
-      <c r="F53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54">
-        <v>2</v>
-      </c>
-      <c r="E54">
-        <v>2</v>
-      </c>
-      <c r="F54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55">
-        <v>2</v>
-      </c>
-      <c r="E55">
-        <v>2</v>
-      </c>
-      <c r="F55">
         <v>2</v>
       </c>
     </row>

</xml_diff>